<commit_message>
correção do parâmetro spb para ano base 2021
</commit_message>
<xml_diff>
--- a/inst/dados_premissas/2021/spb.xlsx
+++ b/inst/dados_premissas/2021/spb.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEC4607F-576C-447A-ABAE-0FD53482C56B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{302EF623-7657-4C6F-B98C-684E2C56A92B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meses" sheetId="3" r:id="rId1"/>
@@ -376,15 +376,15 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -392,7 +392,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -400,7 +400,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -408,7 +408,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -416,15 +416,15 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -445,9 +445,9 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -455,7 +455,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -464,7 +464,7 @@
         <v>0.97499999999999998</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -473,7 +473,7 @@
         <v>0.97499999999999998</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -482,16 +482,16 @@
         <v>0.97499999999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5">
         <f>1-meses!B5/12</f>
-        <v>0.9916666666666667</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+        <v>0.97499999999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>6</v>
       </c>

</xml_diff>